<commit_message>
Weiterführung Unittesting Excel, Refactoring Excelkorrektur
</commit_message>
<xml_diff>
--- a/test/resources/spreadsheet/schullandheim/Aufgabe_Schullandheim.xlsx
+++ b/test/resources/spreadsheet/schullandheim/Aufgabe_Schullandheim.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\VBOXSVR\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="28800" tabRatio="459"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="28800" tabRatio="459" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Einführung" sheetId="1" r:id="rId1"/>
@@ -2021,7 +2021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData>
@@ -3640,7 +3640,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L17:L20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData>
@@ -3761,19 +3763,10 @@
         <v>350</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="25">
-        <f>D17/$E$14</f>
-        <v>12.5</v>
-      </c>
+      <c r="F17" s="25"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="25">
-        <f>F17</f>
-        <v>12.5</v>
-      </c>
-      <c r="L17" s="26">
-        <f>H17*$E$14</f>
-        <v>350</v>
-      </c>
+      <c r="H17" s="25"/>
+      <c r="L17" s="26"/>
     </row>
     <row r="18" spans="1:12" ht="13.5" thickBot="1">
       <c r="A18" s="7" t="s">
@@ -3785,19 +3778,10 @@
         <v>325</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="F18" s="25">
-        <f t="shared" ref="F18:H20" si="0">D18/$E$14</f>
-        <v>11.607142857142858</v>
-      </c>
+      <c r="F18" s="25"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="25">
-        <f>F18*1.1</f>
-        <v>12.767857142857144</v>
-      </c>
-      <c r="L18" s="26">
-        <f t="shared" ref="L18:L20" si="1">H18*$E$14</f>
-        <v>357.50000000000006</v>
-      </c>
+      <c r="H18" s="25"/>
+      <c r="L18" s="26"/>
     </row>
     <row r="19" spans="1:12" ht="13.5" thickBot="1">
       <c r="A19" s="7" t="s">
@@ -3809,19 +3793,10 @@
         <v>370</v>
       </c>
       <c r="E19" s="7"/>
-      <c r="F19" s="25">
-        <f t="shared" si="0"/>
-        <v>13.214285714285714</v>
-      </c>
+      <c r="F19" s="25"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="25">
-        <f>F19*0.85</f>
-        <v>11.232142857142856</v>
-      </c>
-      <c r="L19" s="26">
-        <f t="shared" si="1"/>
-        <v>314.49999999999994</v>
-      </c>
+      <c r="H19" s="25"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="20" spans="1:12" ht="13.5" thickBot="1">
       <c r="A20" s="7" t="s">
@@ -3834,18 +3809,12 @@
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="25">
-        <f t="shared" si="0"/>
-        <v>12.142857142857142</v>
+        <f>D19/$E$14</f>
+        <v>13.214285714285714</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="25">
-        <f t="shared" ref="H18:H20" si="2">F20</f>
-        <v>12.142857142857142</v>
-      </c>
-      <c r="L20" s="26">
-        <f t="shared" si="1"/>
-        <v>340</v>
-      </c>
+      <c r="H20" s="25"/>
+      <c r="L20" s="26"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="7"/>
@@ -4168,12 +4137,12 @@
       </c>
       <c r="D17" s="22">
         <f>F17*$G$16</f>
-        <v>314.49999999999994</v>
+        <v>0</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="22">
         <f>Anreise!H19</f>
-        <v>11.232142857142856</v>
+        <v>0</v>
       </c>
       <c r="H17" s="23"/>
     </row>
@@ -4182,7 +4151,7 @@
         <v>159</v>
       </c>
       <c r="D18" s="22">
-        <f t="shared" ref="D18:D19" si="0">F18*$G$16</f>
+        <f t="shared" ref="D18" si="0">F18*$G$16</f>
         <v>910</v>
       </c>
       <c r="E18" s="7"/>
@@ -4198,12 +4167,12 @@
       </c>
       <c r="D19" s="22">
         <f>SUM(D17:D18)</f>
-        <v>1224.5</v>
+        <v>910</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="22">
         <f>SUM(F17:F18)</f>
-        <v>43.732142857142854</v>
+        <v>32.5</v>
       </c>
       <c r="H19" s="23"/>
     </row>

</xml_diff>